<commit_message>
Changed the file name of FR file
</commit_message>
<xml_diff>
--- a/data-raw/Example_data_sheet_M1.xlsx
+++ b/data-raw/Example_data_sheet_M1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A312A14-8D9C-403B-A497-26797051836C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A464124-356F-4276-959C-BDC4DDCC2951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="52">
   <si>
     <r>
       <rPr>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>Executive Assistant</t>
-  </si>
-  <si>
-    <t>Head of division, board member</t>
   </si>
   <si>
     <t>Receptionist</t>
@@ -1768,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14">
         <v>6</v>
@@ -2457,7 +2454,7 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G27">
         <v>6</v>
@@ -2510,7 +2507,7 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G28">
         <v>3</v>
@@ -2616,7 +2613,7 @@
         <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30">
         <v>7</v>
@@ -2828,7 +2825,7 @@
         <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G34">
         <v>6</v>
@@ -2881,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G35">
         <v>6</v>
@@ -3093,7 +3090,7 @@
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G39">
         <v>7</v>
@@ -3305,7 +3302,7 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G43">
         <v>4</v>
@@ -3623,7 +3620,7 @@
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G49">
         <v>4</v>
@@ -3729,7 +3726,7 @@
         <v>3</v>
       </c>
       <c r="F51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G51">
         <v>4</v>
@@ -3782,7 +3779,7 @@
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G52">
         <v>7</v>
@@ -4471,7 +4468,7 @@
         <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G65">
         <v>7</v>
@@ -5054,7 +5051,7 @@
         <v>6</v>
       </c>
       <c r="F76" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G76">
         <v>5</v>
@@ -5266,7 +5263,7 @@
         <v>5</v>
       </c>
       <c r="F80" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G80">
         <v>7</v>
@@ -5319,7 +5316,7 @@
         <v>5</v>
       </c>
       <c r="F81" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G81">
         <v>6</v>
@@ -5372,7 +5369,7 @@
         <v>6</v>
       </c>
       <c r="F82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G82">
         <v>4</v>
@@ -5637,7 +5634,7 @@
         <v>6</v>
       </c>
       <c r="F87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G87">
         <v>7</v>
@@ -5743,7 +5740,7 @@
         <v>6</v>
       </c>
       <c r="F89" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G89">
         <v>6</v>
@@ -5849,7 +5846,7 @@
         <v>8</v>
       </c>
       <c r="F91" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G91">
         <v>7</v>
@@ -5955,7 +5952,7 @@
         <v>8</v>
       </c>
       <c r="F93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G93">
         <v>5</v>
@@ -6008,7 +6005,7 @@
         <v>3</v>
       </c>
       <c r="F94" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G94">
         <v>6</v>
@@ -6061,7 +6058,7 @@
         <v>5</v>
       </c>
       <c r="F95" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G95">
         <v>5</v>
@@ -6167,7 +6164,7 @@
         <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G97">
         <v>7</v>
@@ -6379,7 +6376,7 @@
         <v>5</v>
       </c>
       <c r="F101" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G101">
         <v>4</v>
@@ -6485,7 +6482,7 @@
         <v>2</v>
       </c>
       <c r="F103" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G103">
         <v>3</v>
@@ -6697,7 +6694,7 @@
         <v>8</v>
       </c>
       <c r="F107" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G107">
         <v>7</v>
@@ -7492,7 +7489,7 @@
         <v>3</v>
       </c>
       <c r="F122" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G122">
         <v>4</v>
@@ -7651,7 +7648,7 @@
         <v>8</v>
       </c>
       <c r="F125" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G125">
         <v>5</v>
@@ -7757,7 +7754,7 @@
         <v>3</v>
       </c>
       <c r="F127" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G127">
         <v>4</v>
@@ -8075,7 +8072,7 @@
         <v>3</v>
       </c>
       <c r="F133" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G133">
         <v>4</v>
@@ -8605,7 +8602,7 @@
         <v>6</v>
       </c>
       <c r="F143" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G143">
         <v>7</v>
@@ -8711,7 +8708,7 @@
         <v>6</v>
       </c>
       <c r="F145" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G145">
         <v>6</v>
@@ -9082,7 +9079,7 @@
         <v>2</v>
       </c>
       <c r="F152" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G152">
         <v>4</v>
@@ -9824,7 +9821,7 @@
         <v>8</v>
       </c>
       <c r="F166" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G166">
         <v>7</v>
@@ -9930,7 +9927,7 @@
         <v>8</v>
       </c>
       <c r="F168" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G168">
         <v>7</v>
@@ -10036,7 +10033,7 @@
         <v>6</v>
       </c>
       <c r="F170" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G170">
         <v>6</v>
@@ -10248,7 +10245,7 @@
         <v>8</v>
       </c>
       <c r="F174" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G174">
         <v>7</v>
@@ -10301,7 +10298,7 @@
         <v>6</v>
       </c>
       <c r="F175" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G175">
         <v>4</v>
@@ -10460,7 +10457,7 @@
         <v>3</v>
       </c>
       <c r="F178" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G178">
         <v>4</v>
@@ -11096,7 +11093,7 @@
         <v>5</v>
       </c>
       <c r="F190" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G190">
         <v>7</v>
@@ -11414,7 +11411,7 @@
         <v>8</v>
       </c>
       <c r="F196" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I196">
         <v>100</v>
@@ -11461,7 +11458,7 @@
         <v>8</v>
       </c>
       <c r="F197" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G197">
         <v>4</v>
@@ -11779,7 +11776,7 @@
         <v>6</v>
       </c>
       <c r="F203" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G203">
         <v>5</v>
@@ -11991,7 +11988,7 @@
         <v>6</v>
       </c>
       <c r="F207" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G207">
         <v>6</v>
@@ -12097,7 +12094,7 @@
         <v>5</v>
       </c>
       <c r="F209" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G209">
         <v>4</v>
@@ -12256,7 +12253,7 @@
         <v>6</v>
       </c>
       <c r="F212" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G212">
         <v>4</v>
@@ -12468,7 +12465,7 @@
         <v>8</v>
       </c>
       <c r="F216" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G216">
         <v>7</v>
@@ -12733,7 +12730,7 @@
         <v>5</v>
       </c>
       <c r="F221" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G221">
         <v>4</v>
@@ -12839,7 +12836,7 @@
         <v>6</v>
       </c>
       <c r="F223" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G223">
         <v>6</v>
@@ -12892,7 +12889,7 @@
         <v>3</v>
       </c>
       <c r="F224" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G224">
         <v>6</v>
@@ -12998,7 +12995,7 @@
         <v>8</v>
       </c>
       <c r="F226" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G226">
         <v>7</v>
@@ -13104,7 +13101,7 @@
         <v>6</v>
       </c>
       <c r="F228" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G228">
         <v>4</v>
@@ -13263,7 +13260,7 @@
         <v>8</v>
       </c>
       <c r="F231" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I231">
         <v>100</v>
@@ -13681,7 +13678,7 @@
         <v>6</v>
       </c>
       <c r="F239" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G239">
         <v>4</v>
@@ -13734,7 +13731,7 @@
         <v>2</v>
       </c>
       <c r="F240" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G240">
         <v>3</v>
@@ -13787,7 +13784,7 @@
         <v>3</v>
       </c>
       <c r="F241" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G241">
         <v>4</v>
@@ -13840,7 +13837,7 @@
         <v>6</v>
       </c>
       <c r="F242" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G242">
         <v>6</v>
@@ -14052,7 +14049,7 @@
         <v>1</v>
       </c>
       <c r="F246" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G246">
         <v>3</v>
@@ -14105,7 +14102,7 @@
         <v>8</v>
       </c>
       <c r="F247" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G247">
         <v>7</v>
@@ -14158,7 +14155,7 @@
         <v>2</v>
       </c>
       <c r="F248" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G248">
         <v>4</v>
@@ -14423,7 +14420,7 @@
         <v>2</v>
       </c>
       <c r="F253" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G253">
         <v>5</v>
@@ -14582,7 +14579,7 @@
         <v>8</v>
       </c>
       <c r="F256" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I256">
         <v>100</v>
@@ -14629,7 +14626,7 @@
         <v>8</v>
       </c>
       <c r="F257" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I257">
         <v>100</v>
@@ -15047,7 +15044,7 @@
         <v>6</v>
       </c>
       <c r="F265" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G265">
         <v>5</v>
@@ -15100,7 +15097,7 @@
         <v>6</v>
       </c>
       <c r="F266" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G266">
         <v>6</v>
@@ -15206,7 +15203,7 @@
         <v>6</v>
       </c>
       <c r="F268" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G268">
         <v>4</v>
@@ -15418,7 +15415,7 @@
         <v>6</v>
       </c>
       <c r="F272" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G272">
         <v>4</v>
@@ -15842,7 +15839,7 @@
         <v>6</v>
       </c>
       <c r="F280" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G280">
         <v>6</v>
@@ -15948,7 +15945,7 @@
         <v>6</v>
       </c>
       <c r="F282" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G282">
         <v>6</v>
@@ -16054,7 +16051,7 @@
         <v>1</v>
       </c>
       <c r="F284" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I284">
         <v>100</v>
@@ -16154,7 +16151,7 @@
         <v>6</v>
       </c>
       <c r="F286" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G286">
         <v>6</v>

</xml_diff>